<commit_message>
Doku und Zeitliste Gergely angepasst
</commit_message>
<xml_diff>
--- a/Zeitleisten/Gergely_zeitliste.xlsx
+++ b/Zeitleisten/Gergely_zeitliste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\ESE Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\ese-project\Zeitleisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6C2B21F-059F-428D-B19E-96B0998B447E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{21F72D50-52D0-4A44-952B-E0B104F6DBDB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="4470" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Datum</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Abstimmung Embedded Integration</t>
+  </si>
+  <si>
+    <t>Recherche und Implementierungsversuche CRC</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C141"/>
+  <dimension ref="A1:C143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1028,21 +1031,21 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43262</v>
+        <v>43261</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43268</v>
+        <v>43261</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -1050,21 +1053,21 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43269</v>
+        <v>43262</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43280</v>
+        <v>43268</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -1072,10 +1075,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43280</v>
+        <v>43269</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1086,7 +1089,7 @@
         <v>43280</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -1097,7 +1100,7 @@
         <v>43280</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -1108,7 +1111,7 @@
         <v>43280</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -1116,24 +1119,24 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43281</v>
+        <v>43280</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43281</v>
+        <v>43280</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1141,10 +1144,10 @@
         <v>43281</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1152,10 +1155,10 @@
         <v>43281</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1163,7 +1166,7 @@
         <v>43281</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -1174,7 +1177,7 @@
         <v>43281</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -1182,10 +1185,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43282</v>
+        <v>43281</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -1193,10 +1196,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>43282</v>
+        <v>43281</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -1218,7 +1221,7 @@
         <v>43282</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -1229,7 +1232,7 @@
         <v>43282</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -1237,33 +1240,55 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
         <v>43283</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>23</v>
       </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="7"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B60" s="6" t="s">
+      <c r="C60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="7"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B62" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C60">
-        <f>SUM($C2:$C58)</f>
-        <v>104</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" s="8" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="1"/>
-      <c r="B141"/>
-      <c r="C141"/>
+      <c r="C62">
+        <f>SUM($C2:$C60)</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" s="8" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="1"/>
+      <c r="B143"/>
+      <c r="C143"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>